<commit_message>
Version 3.0.1 neue optionen @keyselection, @selection und verbesserte EDPSession-Handling
</commit_message>
<xml_diff>
--- a/src/main/resources/base/owfw7/TestCustomer.xlsx
+++ b/src/main/resources/base/owfw7/TestCustomer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkellermann.ABASAG\git\importitnew\src\main\resources\base\ow1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkellermann\Documents\git\importitnew\src\main\resources\base\owfw7\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -186,9 +186,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <charset val="204"/>
     </font>
@@ -210,13 +217,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -563,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -574,9 +584,10 @@
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -584,7 +595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -606,8 +617,9 @@
       <c r="G2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -630,7 +642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -653,7 +665,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -676,7 +688,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -699,7 +711,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -722,7 +734,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -745,7 +757,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -768,7 +780,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>51</v>
       </c>

</xml_diff>